<commit_message>
Added Final Draft (ipynb) to my personal folder
</commit_message>
<xml_diff>
--- a/Data-Arun/Graduation_Rate_5yrs.xlsx
+++ b/Data-Arun/Graduation_Rate_5yrs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aarthi Manoharan\Arun\1 Project Day 1\Activity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aarthi Manoharan\Arun\1 Project Day 1\fintech-project01\Data-Arun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFA6FC3-8B67-4123-9AB5-196A6E6D141D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA10313-AC23-4321-983A-8CFF74202724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CD3B7EDB-FA47-44BC-8D8B-B10A35DDF682}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD3B7EDB-FA47-44BC-8D8B-B10A35DDF682}"/>
   </bookViews>
   <sheets>
     <sheet name="Graduation rate" sheetId="1" r:id="rId1"/>
@@ -258,13 +258,13 @@
     <t>York Region DSB</t>
   </si>
   <si>
-    <t>Board</t>
-  </si>
-  <si>
     <t>Graduation Rate</t>
   </si>
   <si>
     <t>Literacy Test</t>
+  </si>
+  <si>
+    <t>Board Name</t>
   </si>
 </sst>
 </file>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9598AB-7CE2-46CE-878F-7A0C2F663E02}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,10 +681,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1273,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84F9716-09F8-4E4A-953E-32F79BA0225C}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,10 +1285,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>